<commit_message>
Fixed some mysterious bugs
</commit_message>
<xml_diff>
--- a/mag_curvefit.xlsx
+++ b/mag_curvefit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jean/Spring24/bio/BioinspiredRobot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38ACA72-79E7-9F4E-A8E3-B8F936B7D4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C8AB3-664F-A342-A705-7336EA684107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" xr2:uid="{E83E4C41-BBE3-FA4B-9696-42C9A9A69A21}"/>
   </bookViews>
@@ -36,12 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>distance (y dir)</t>
   </si>
   <si>
     <t>magnetometer reading</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>xr</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>zr</t>
+  </si>
+  <si>
+    <t>distr</t>
   </si>
 </sst>
 </file>
@@ -83,9 +107,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +601,896 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.52375738676229833"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2:$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="3">
+                  <c:v>247.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$8:$W$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$8:$Y$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.873000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.089</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.704000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B01-1D40-87BB-2061D667A3E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="446633056"/>
+        <c:axId val="446634784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="446633056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446634784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="446634784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446633056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$K$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>247.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.109</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.66</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.79700000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CC5-B240-9BA9-21FD2E0869EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1344805360"/>
+        <c:axId val="1344856736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1344805360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1344856736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1344856736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1344805360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1131,19 +2046,1051 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1164,6 +3111,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D708C0C5-144D-8242-63C5-325B047848DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>317853</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>134761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>766586</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>32808</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421BEAC1-05E6-5FD8-D56B-D6258F053832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1489,10 +3508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB09FC1-BDE6-FF4E-819B-43CB3C66EE8B}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="168" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1500,7 +3519,7 @@
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,11 +3535,32 @@
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.01</v>
       </c>
@@ -1538,9 +3578,18 @@
       <c r="J2" s="1">
         <v>0.01</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q22" si="0">SQRT(N2^2+O2^2+P2^2)</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U25" si="1">SQRT(R2^2+S2^2+T2^2)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.02</v>
       </c>
@@ -1548,7 +3597,7 @@
         <v>1770.9960000000001</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">LN(B3/3713.4)/(-37.3)</f>
+        <f t="shared" ref="D3:D21" si="2">LN(B3/3713.4)/(-37.3)</f>
         <v>1.9850021415657969E-2</v>
       </c>
       <c r="F3" s="1">
@@ -1558,9 +3607,18 @@
       <c r="J3" s="1">
         <v>0.02</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.03</v>
       </c>
@@ -1568,7 +3626,7 @@
         <v>1155.8889999999999</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1288958555297113E-2</v>
       </c>
       <c r="F4" s="1">
@@ -1578,9 +3636,18 @@
       <c r="J4" s="1">
         <v>0.03</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.04</v>
       </c>
@@ -1588,7 +3655,7 @@
         <v>745.62599999999998</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3042333618373778E-2</v>
       </c>
       <c r="F5" s="1">
@@ -1598,9 +3665,29 @@
       <c r="J5" s="1">
         <v>0.04</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5">
+        <v>4.5</v>
+      </c>
+      <c r="L5">
+        <v>247.5</v>
+      </c>
+      <c r="M5">
+        <v>4.75</v>
+      </c>
+      <c r="N5">
+        <v>385.24</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="Q5" t="e">
+        <f>SQRT(#REF!^2+O5^2+P5^2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.05</v>
       </c>
@@ -1608,7 +3695,7 @@
         <v>506.58</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3405386596887594E-2</v>
       </c>
       <c r="F6" s="1">
@@ -1618,9 +3705,18 @@
       <c r="J6" s="1">
         <v>0.05</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.06</v>
       </c>
@@ -1628,7 +3724,7 @@
         <v>333.846</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4585076921449228E-2</v>
       </c>
       <c r="F7" s="1">
@@ -1638,9 +3734,18 @@
       <c r="J7" s="1">
         <v>0.06</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1648,7 +3753,7 @@
         <v>228.43</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.4757998935806785E-2</v>
       </c>
       <c r="F8" s="1">
@@ -1658,9 +3763,34 @@
       <c r="J8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K8" s="1"/>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>95</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X8">
+        <f>W8*100</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="Y8">
+        <v>71</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.08</v>
       </c>
@@ -1668,7 +3798,7 @@
         <v>157.80099999999999</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.4674756902039197E-2</v>
       </c>
       <c r="F9" s="1">
@@ -1678,9 +3808,28 @@
       <c r="J9" s="1">
         <v>0.08</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>72.2</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ref="X9:X29" si="3">W9*100</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.09</v>
       </c>
@@ -1688,7 +3837,7 @@
         <v>114.29</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.332343431806607E-2</v>
       </c>
       <c r="F10" s="1">
@@ -1698,9 +3847,28 @@
       <c r="J10" s="1">
         <v>0.09</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="2"/>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0.09</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="Y10">
+        <v>35</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.1</v>
       </c>
@@ -1708,7 +3876,7 @@
         <v>81.052999999999997</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.10253619078519897</v>
       </c>
       <c r="F11" s="1">
@@ -1718,9 +3886,28 @@
       <c r="J11" s="1">
         <v>0.1</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11">
+        <v>10.5</v>
+      </c>
+      <c r="L11">
+        <v>49</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.11</v>
       </c>
@@ -1728,7 +3915,7 @@
         <v>58.207000000000001</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1114128030979715</v>
       </c>
       <c r="F12" s="1">
@@ -1738,9 +3925,28 @@
       <c r="J12" s="1">
         <v>0.11</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0.11</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="Y12">
+        <v>18.873000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.12</v>
       </c>
@@ -1748,7 +3954,7 @@
         <v>43.024999999999999</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11951533072052997</v>
       </c>
       <c r="F13" s="1">
@@ -1758,9 +3964,28 @@
       <c r="J13" s="1">
         <v>0.12</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0.12</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Y13">
+        <v>14.089</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.13</v>
       </c>
@@ -1768,7 +3993,7 @@
         <v>32.363999999999997</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12714896740020853</v>
       </c>
       <c r="F14" s="1">
@@ -1778,9 +4003,28 @@
       <c r="J14" s="1">
         <v>0.13</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0.14000000000000001</v>
       </c>
@@ -1788,7 +4032,7 @@
         <v>22.824999999999999</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13651063676923161</v>
       </c>
       <c r="F15" s="1">
@@ -1798,9 +4042,22 @@
       <c r="J15" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.15</v>
       </c>
@@ -1808,7 +4065,7 @@
         <v>17.78</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1432072103991317</v>
       </c>
       <c r="F16" s="1">
@@ -1818,17 +4075,34 @@
       <c r="J16" s="1">
         <v>0.15</v>
       </c>
-      <c r="K16" s="1">
-        <v>56.228000000000002</v>
+      <c r="K16">
+        <v>15.5</v>
       </c>
       <c r="L16">
-        <v>51.411000000000001</v>
-      </c>
-      <c r="M16">
-        <v>72.349999999999994</v>
+        <v>12.96</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0.15</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="Y16">
+        <v>10.704000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.16</v>
       </c>
@@ -1836,7 +4110,7 @@
         <v>11.941000000000001</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1538800354268666</v>
       </c>
       <c r="F17" s="1">
@@ -1846,9 +4120,28 @@
       <c r="J17" s="1">
         <v>0.16</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0.16750000000000001</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="3"/>
+        <v>16.75</v>
+      </c>
+      <c r="Y17">
+        <v>8.06</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.17</v>
       </c>
@@ -1856,7 +4149,7 @@
         <v>8.3149999999999995</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16358289719379304</v>
       </c>
       <c r="F18" s="1">
@@ -1871,9 +4164,22 @@
       <c r="J18" s="1">
         <v>0.17</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.18</v>
       </c>
@@ -1881,7 +4187,7 @@
         <v>4.6050000000000004</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17942521469882308</v>
       </c>
       <c r="F19" s="1">
@@ -1893,9 +4199,30 @@
       <c r="J19" s="1">
         <v>0.18</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1">
+        <v>18.25</v>
+      </c>
+      <c r="L19" s="1">
+        <v>9.109</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.19</v>
       </c>
@@ -1903,7 +4230,7 @@
         <v>2.5209999999999999</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19557768176320614</v>
       </c>
       <c r="F20" s="1">
@@ -1918,9 +4245,35 @@
       <c r="J20" s="1">
         <v>0.19</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1">
+        <v>19.25</v>
+      </c>
+      <c r="L20" s="1">
+        <v>7.66</v>
+      </c>
+      <c r="N20" s="1">
+        <v>10</v>
+      </c>
+      <c r="O20" s="1">
+        <v>29.024999999999999</v>
+      </c>
+      <c r="P20" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>31.02741731114596</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.2</v>
       </c>
@@ -1928,7 +4281,7 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22453587348026183</v>
       </c>
       <c r="F21" s="1">
@@ -1943,14 +4296,220 @@
       <c r="J21" s="1">
         <v>0.2</v>
       </c>
-      <c r="K21" s="1">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="M21" s="1">
-        <v>1.4</v>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J22" s="1">
+        <f>J21+0.01</f>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0.21</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="Y22">
+        <v>4.5110000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J23" s="1">
+        <f t="shared" ref="J23:J31" si="4">J22+0.01</f>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="K23">
+        <v>22.75</v>
+      </c>
+      <c r="L23">
+        <v>4.1310000000000002</v>
+      </c>
+      <c r="N23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>22.5</v>
+      </c>
+      <c r="P23">
+        <f>3.25+2</f>
+        <v>5.25</v>
+      </c>
+      <c r="Q23">
+        <f>SQRT(N23^2+O23^2+P23^2)</f>
+        <v>24.141509894784956</v>
+      </c>
+      <c r="R23">
+        <v>4.5369999999999999</v>
+      </c>
+      <c r="S23">
+        <v>11.925000000000001</v>
+      </c>
+      <c r="T23">
+        <v>-2.246</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="1"/>
+        <v>12.955095908560462</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J24" s="1">
+        <f t="shared" si="4"/>
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="Q24">
+        <f>SQRT(N24^2+O24^2+P24^2)</f>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0.23</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="Y24">
+        <v>3.5830000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J25" s="1">
+        <f t="shared" si="4"/>
+        <v>0.24000000000000005</v>
+      </c>
+      <c r="Q25">
+        <f>SQRT(N25^2+O25^2+P25^2)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="3"/>
+      <c r="U25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J26" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="N26">
+        <v>7.75</v>
+      </c>
+      <c r="O26">
+        <v>26.5</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <f>SQRT(N26^2+O26^2+P26^2)</f>
+        <v>28.059089436401887</v>
+      </c>
+      <c r="R26">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="S26">
+        <v>-0.19</v>
+      </c>
+      <c r="T26">
+        <v>-1.63</v>
+      </c>
+      <c r="U26">
+        <f>SQRT(R26^2+S26^2+T26^2)</f>
+        <v>1.6410679571547302</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J27" s="1">
+        <f t="shared" si="4"/>
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J28" s="1">
+        <f t="shared" si="4"/>
+        <v>0.27000000000000007</v>
+      </c>
+      <c r="K28">
+        <v>27</v>
+      </c>
+      <c r="L28">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J29" s="1">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000008</v>
+      </c>
+      <c r="W29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="3"/>
+        <v>28.000000000000004</v>
+      </c>
+      <c r="Y29">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J30" s="1">
+        <f t="shared" si="4"/>
+        <v>0.29000000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J31" s="1">
+        <f t="shared" si="4"/>
+        <v>0.3000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>